<commit_message>
adding addition to excel
</commit_message>
<xml_diff>
--- a/aci/data/data.xlsx
+++ b/aci/data/data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\dev\Netops\aci\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\repo\Netops\aci\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518A6335-CE5A-48CA-B6E9-B2A26B97DC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5D065D-72BC-4FF5-B184-C7CEFC852E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="1140" windowWidth="18135" windowHeight="11430" xr2:uid="{F54781CD-7594-437D-A5FD-688F83CAA78E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{F54781CD-7594-437D-A5FD-688F83CAA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="RegisterNodes" sheetId="1" r:id="rId1"/>
+    <sheet name="Variables" sheetId="2" r:id="rId2"/>
+    <sheet name="test" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>APIC</t>
   </si>
@@ -88,6 +90,21 @@
   </si>
   <si>
     <t>FakeLeaf-233</t>
+  </si>
+  <si>
+    <t>Tenant Name</t>
+  </si>
+  <si>
+    <t>Apic Address</t>
+  </si>
+  <si>
+    <t>TestTenantName</t>
+  </si>
+  <si>
+    <t>Apic</t>
+  </si>
+  <si>
+    <t>Tenant</t>
   </si>
 </sst>
 </file>
@@ -447,20 +464,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661BDB76-38E8-4702-AE2A-8B0217D00A82}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.86328125" customWidth="1"/>
-    <col min="3" max="3" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="23.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -494,7 +511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -511,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -528,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -545,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -562,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -586,4 +603,109 @@
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 This document is protected by Altron - labelled as General Business Information</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39E1C27F-2C00-49FD-AEC7-2490647B71B6}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1151655C-DC50-4A71-A26B-6B01F738779A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{702B6C99-CCEE-4940-BDF3-84B5BC620C36}">
+          <x14:formula1>
+            <xm:f>Variables!$C$2:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>C3:C14</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E7148A1D-A865-4289-96EB-215511469B80}">
+          <x14:formula1>
+            <xm:f>Variables!$C$2:$C$22</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3FF82987-4C73-486B-93F9-56C1DCBA32CC}">
+          <x14:formula1>
+            <xm:f>Variables!$B$2:$B$60</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{99AA599D-9032-46B2-9749-C907BA390598}">
+          <x14:formula1>
+            <xm:f>Variables!$A$2:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>